<commit_message>
accrual periodicity graphics chart pie & bar label
</commit_message>
<xml_diff>
--- a/test/result/result.xlsx
+++ b/test/result/result.xlsx
@@ -181,6 +181,90 @@
       </nvPicPr>
       <blipFill>
         <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>12</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="9525000" cy="6667500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>25</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="9525000" cy="6667500"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId3"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>37</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6096000" cy="4572000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="4" name="Image 4" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId4"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -483,7 +567,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,896 +610,1659 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>https://datos.hcdn.gob.ar/</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
+          <t>https://transparencia.enargas.gob.ar/data.json</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">None is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Bloques, Interbloques e Integración</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>1</v>
+          <t>Reclamos resueltos por las Distribuidoras de gas natural</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t xml:space="preserve">'superTheme' is a required property &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>https://datos.hcdn.gob.ar/</t>
-        </is>
-      </c>
-      <c r="B3" t="b">
-        <v>1</v>
+          <t>https://transparencia.enargas.gob.ar/data.json</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve">None is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Comisiones</t>
-        </is>
-      </c>
-      <c r="E3" t="b">
-        <v>1</v>
+          <t>Reclamos resueltos por el ENARGAS</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t xml:space="preserve">'superTheme' is a required property &amp;&amp; 'http://www4.hcdn.gob.ar/Datos_doc/DOCUMENTACION – COMISIONES.pdf' is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>https://datos.hcdn.gob.ar/</t>
-        </is>
-      </c>
-      <c r="B4" t="b">
-        <v>1</v>
+          <t>https://datos.arsat.com.ar/data.json</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve">None is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Diarios de Sesiones</t>
-        </is>
-      </c>
-      <c r="E4" t="b">
-        <v>1</v>
+          <t>Personal</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t xml:space="preserve">'superTheme' is a required property &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>https://datos.hcdn.gob.ar/</t>
-        </is>
-      </c>
-      <c r="B5" t="b">
-        <v>1</v>
+          <t>https://datos.arsat.com.ar/data.json</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t xml:space="preserve">None is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Dictamenes</t>
-        </is>
-      </c>
-      <c r="E5" t="b">
-        <v>1</v>
+          <t>Cine.Ar Play</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t xml:space="preserve">'superTheme' is a required property &amp;&amp; 'accrualPeriodicity' is a required property &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>https://datos.hcdn.gob.ar/</t>
-        </is>
-      </c>
-      <c r="B6" t="b">
-        <v>1</v>
+          <t>https://datos.arsat.com.ar/data.json</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve">None is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Dietas y Gastos de Representación - Legisladores/as</t>
-        </is>
-      </c>
-      <c r="E6" t="b">
-        <v>1</v>
+          <t>Ejecuciones presupuestarias</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t xml:space="preserve">'superTheme' is a required property &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>https://datos.hcdn.gob.ar/</t>
-        </is>
-      </c>
-      <c r="B7" t="b">
-        <v>1</v>
+          <t>https://datos.arsat.com.ar/data.json</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve">None is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Ejecución Presupuestaria de la Cámara de Diputados de la Nación</t>
-        </is>
-      </c>
-      <c r="E7" t="b">
-        <v>1</v>
+          <t>Finanzas</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t xml:space="preserve">'superTheme' is a required property &amp;&amp; 'http://www4.hcdn.gob.ar/Datos_doc/Documentación Ejecución Presupuestaria.pdf' is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>https://datos.hcdn.gob.ar/</t>
-        </is>
-      </c>
-      <c r="B8" t="b">
-        <v>1</v>
+          <t>https://datos.arsat.com.ar/data.json</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve">None is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Escala Salarial</t>
-        </is>
-      </c>
-      <c r="E8" t="b">
-        <v>1</v>
+          <t>Servicio REFEFO</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t xml:space="preserve">'superTheme' is a required property &amp;&amp; 'http://www4.hcdn.gob.ar/Datos_doc/Doc Escala Salarial.pdf' is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>https://datos.hcdn.gob.ar/</t>
-        </is>
-      </c>
-      <c r="B9" t="b">
-        <v>1</v>
+          <t>https://datos.arsat.com.ar/data.json</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">None is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Estructura orgánica de la Cámara de Diputados de la Nación</t>
-        </is>
-      </c>
-      <c r="E9" t="b">
-        <v>1</v>
+          <t>Puntos de conexión REFEFO</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t xml:space="preserve">'superTheme' is a required property &amp;&amp; 'http://www4.hcdn.gob.ar/Datos_doc/Doc Estructura Orgánica.pdf' is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>https://datos.hcdn.gob.ar/</t>
-        </is>
-      </c>
-      <c r="B10" t="b">
-        <v>1</v>
+          <t>https://datos.arsat.com.ar/data.json</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve">None is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Estructura orgánica de la Cámara de Diputados de la Nación</t>
-        </is>
-      </c>
-      <c r="E10" t="b">
-        <v>1</v>
+          <t>Cobertura Satélite ARSAT-2</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t xml:space="preserve">'superTheme' is a required property &amp;&amp; 'accrualPeriodicity' is a required property &amp;&amp; '' is too short &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>https://datos.hcdn.gob.ar/</t>
-        </is>
-      </c>
-      <c r="B11" t="b">
-        <v>1</v>
+          <t>https://datos.arsat.com.ar/data.json</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve">None is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Expedientes</t>
-        </is>
-      </c>
-      <c r="E11" t="b">
-        <v>1</v>
+          <t>Cobertura Satélite ARSAT-1</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t xml:space="preserve">'superTheme' is a required property &amp;&amp; 'accrualPeriodicity' is a required property &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>https://datos.hcdn.gob.ar/</t>
-        </is>
-      </c>
-      <c r="B12" t="b">
-        <v>1</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">None is not valid under any of the given schemas &amp;&amp; </t>
+          <t>https://monitoreo.datos.gob.ar/catalog/jgm/data.json</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>No</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Firmantes Leyes Sancionadas</t>
-        </is>
-      </c>
-      <c r="E12" t="b">
-        <v>1</v>
+          <t>Registro Legajo Multipropósito - RLM</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t xml:space="preserve">'superTheme' is a required property &amp;&amp; 'http://www4.hcdn.gob.ar/Datos_doc/Doc_Firmantes leyes sancionadas.pdf' is not valid under any of the given schemas &amp;&amp; </t>
+          <t xml:space="preserve">'accessURL' is a required property &amp;&amp; </t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>https://datos.hcdn.gob.ar/</t>
-        </is>
-      </c>
-      <c r="B13" t="b">
-        <v>1</v>
+          <t>https://monitoreo.datos.gob.ar/catalog/aaip/data.json</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve">None is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Giro a Comisiones</t>
-        </is>
-      </c>
-      <c r="E13" t="b">
-        <v>1</v>
+          <t>Solicitudes de acceso a la información pública</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t xml:space="preserve">'superTheme' is a required property &amp;&amp; 'accrualPeriodicity' is a required property &amp;&amp; 'http://www4.hcdn.gob.ar/Datos_doc/Documentacion-giro comisiones.pdf' is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>https://datos.hcdn.gob.ar/</t>
-        </is>
-      </c>
-      <c r="B14" t="b">
-        <v>1</v>
+          <t>https://monitoreo.datos.gob.ar/catalog/aaip/data.json</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t xml:space="preserve">None is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Grupos Parlamentarios de Amistad</t>
-        </is>
-      </c>
-      <c r="E14" t="b">
-        <v>1</v>
+          <t>Reclamos sobre solicitudes de acceso a la información pública</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t xml:space="preserve">'superTheme' is a required property &amp;&amp; 'http://www4.hcdn.gob.ar/Datos_doc/Doc Grupos Parlamentarios de Amistad.pdf' is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>https://datos.hcdn.gob.ar/</t>
-        </is>
-      </c>
-      <c r="B15" t="b">
-        <v>1</v>
+          <t>http://monitoreo.datos.gob.ar/catalog/otros/data.json</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t xml:space="preserve">None is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Diputados</t>
-        </is>
-      </c>
-      <c r="E15" t="b">
-        <v>1</v>
+          <t>Solicitudes de Acceso a la Información Pública (2015 y 2016)</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t xml:space="preserve">'superTheme' is a required property &amp;&amp; 'http://www4.hcdn.gob.ar/Datos_doc/DOCUMENTACION – DIPUTADOS.pdf' is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="inlineStr">
         <is>
-          <t>https://datos.hcdn.gob.ar/</t>
-        </is>
-      </c>
-      <c r="B16" t="b">
-        <v>1</v>
+          <t>http://monitoreo.datos.gob.ar/catalog/otros/data.json</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t xml:space="preserve">None is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Leyes Promulgadas</t>
-        </is>
-      </c>
-      <c r="E16" t="b">
-        <v>1</v>
+          <t>Nombres de personas físicas</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t xml:space="preserve">'superTheme' is a required property &amp;&amp; 'http://www4.hcdn.gob.ar/Datos_doc/DOCUMENTACION – LEYESPRMULGADAS.pdf' is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>https://datos.hcdn.gob.ar/</t>
-        </is>
-      </c>
-      <c r="B17" t="b">
-        <v>1</v>
+          <t>http://monitoreo.datos.gob.ar/catalog/otros/data.json</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t xml:space="preserve">None is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Leyes Sancionadas</t>
-        </is>
-      </c>
-      <c r="E17" t="b">
-        <v>1</v>
+          <t>Resultados Electorales 2015</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t xml:space="preserve">'superTheme' is a required property &amp;&amp; 'accrualPeriodicity' is a required property &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="inlineStr">
         <is>
-          <t>https://datos.hcdn.gob.ar/</t>
-        </is>
-      </c>
-      <c r="B18" t="b">
-        <v>1</v>
+          <t>http://monitoreo.datos.gob.ar/catalog/otros/data.json</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t xml:space="preserve">None is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Sumario de leyes</t>
-        </is>
-      </c>
-      <c r="E18" t="b">
-        <v>1</v>
+          <t>Resultados Provisorios  Elecciones Primarias, Abiertas, Simultáneas y Obligatorias (PASO) 2019</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t xml:space="preserve">'superTheme' is a required property &amp;&amp; 'accrualPeriodicity' is a required property &amp;&amp; 'http://www4.hcdn.gob.ar/Datos_doc/DOCUMENTACION – SUMARIO LEYES.pdf' is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>https://datos.hcdn.gob.ar/</t>
-        </is>
-      </c>
-      <c r="B19" t="b">
-        <v>1</v>
+          <t>http://monitoreo.datos.gob.ar/catalog/otros/data.json</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t xml:space="preserve">None is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Licitaciones y Contrataciones</t>
-        </is>
-      </c>
-      <c r="E19" t="b">
-        <v>1</v>
+          <t>Inmuebles Propios del Estado Nacional y Alquilados</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t xml:space="preserve">'superTheme' is a required property &amp;&amp; 'http://www4.hcdn.gob.ar/Datos_doc/Documentación Licitaciones y Contrataciones.pdf' is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="inlineStr">
         <is>
-          <t>https://datos.hcdn.gob.ar/</t>
-        </is>
-      </c>
-      <c r="B20" t="b">
-        <v>1</v>
+          <t>http://monitoreo.datos.gob.ar/catalog/otros/data.json</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t xml:space="preserve">None is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Misiones Oficiales</t>
-        </is>
-      </c>
-      <c r="E20" t="b">
-        <v>1</v>
+          <t>Contratos de Alquiler del Estado Nacional como Locador</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t xml:space="preserve">'superTheme' is a required property &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>https://datos.hcdn.gob.ar/</t>
-        </is>
-      </c>
-      <c r="B21" t="b">
-        <v>1</v>
+          <t>http://monitoreo.datos.gob.ar/catalog/otros/data.json</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t xml:space="preserve">None is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Movimientos de proyectos</t>
-        </is>
-      </c>
-      <c r="E21" t="b">
-        <v>1</v>
+          <t>Registro Único de Audiencias de Gestión de Intereses</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t xml:space="preserve">'superTheme' is a required property &amp;&amp; 'accrualPeriodicity' is a required property &amp;&amp; 'http://www4.hcdn.gob.ar/Datos_doc/Documentacion-movimientos proyectos .pdf' is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>https://datos.hcdn.gob.ar/</t>
-        </is>
-      </c>
-      <c r="B22" t="b">
-        <v>1</v>
+          <t>http://monitoreo.datos.gob.ar/catalog/otros/data.json</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t xml:space="preserve">None is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Nómina de personal</t>
-        </is>
-      </c>
-      <c r="E22" t="b">
-        <v>1</v>
+          <t>Resultados Provisorios Elecciones Generales 2019</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t xml:space="preserve">'superTheme' is a required property &amp;&amp; 'http://www4.hcdn.gob.ar/Datos_doc/Documentación Nómina de Personal.pdf' is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>https://datos.hcdn.gob.ar/</t>
-        </is>
-      </c>
-      <c r="B23" t="b">
-        <v>1</v>
+          <t>http://monitoreo.datos.gob.ar/catalog/otros/data.json</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t xml:space="preserve">None is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Periodos Parlamentarios</t>
-        </is>
-      </c>
-      <c r="E23" t="b">
-        <v>1</v>
+          <t>Índice de Tipo de Cambio Real Sectorial Efectivo - Discontinuado</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t xml:space="preserve">'superTheme' is a required property &amp;&amp; 'accrualPeriodicity' is a required property &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="inlineStr">
         <is>
-          <t>https://datos.hcdn.gob.ar/</t>
-        </is>
-      </c>
-      <c r="B24" t="b">
-        <v>1</v>
+          <t>http://monitoreo.datos.gob.ar/catalog/otros/data.json</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t xml:space="preserve">None is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Proyectos Parlamentarios</t>
-        </is>
-      </c>
-      <c r="E24" t="b">
-        <v>1</v>
+          <t>Indicador de Importaciones de Bienes de Capital Productivo - Discontinuado</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t xml:space="preserve">'superTheme' is a required property &amp;&amp; 'http://www4.hcdn.gob.ar/Datos_doc/DOCUMENTACION - PROYECTOS PARLAMENTARIOS.pdf' is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>https://datos.hcdn.gob.ar/</t>
-        </is>
-      </c>
-      <c r="B25" t="b">
-        <v>1</v>
+          <t>http://monitoreo.datos.gob.ar/catalog/otros/data.json</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t xml:space="preserve">None is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Publicaciones</t>
-        </is>
-      </c>
-      <c r="E25" t="b">
-        <v>1</v>
+          <t>Indicadores de Empleo de Trabajadores Registrados (OEDE) - Discontinuado</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t xml:space="preserve">'superTheme' is a required property &amp;&amp; 'http://www4.hcdn.gob.ar/Datos_doc/DOCUMENTACION – PUBLICACIONES.pdf' is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="inlineStr">
         <is>
-          <t>https://datos.hcdn.gob.ar/</t>
-        </is>
-      </c>
-      <c r="B26" t="b">
-        <v>1</v>
+          <t>http://monitoreo.datos.gob.ar/catalog/otros/data.json</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t xml:space="preserve">None is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Redes Sociales</t>
-        </is>
-      </c>
-      <c r="E26" t="b">
-        <v>1</v>
+          <t>Indicadores de Remuneraciones de Trabajadores Registrados (OEDE) - Discontinuado</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t xml:space="preserve">'superTheme' is a required property &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="inlineStr">
         <is>
-          <t>https://datos.hcdn.gob.ar/</t>
-        </is>
-      </c>
-      <c r="B27" t="b">
-        <v>1</v>
+          <t>http://monitoreo.datos.gob.ar/catalog/otros/data.json</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t xml:space="preserve">None is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Resultado de proyectos</t>
-        </is>
-      </c>
-      <c r="E27" t="b">
-        <v>1</v>
+          <t>Ahora 12 - Discontinuado</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t xml:space="preserve">'superTheme' is a required property &amp;&amp; 'accrualPeriodicity' is a required property &amp;&amp; '' is too short &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="inlineStr">
         <is>
-          <t>https://datos.hcdn.gob.ar/</t>
-        </is>
-      </c>
-      <c r="B28" t="b">
-        <v>1</v>
+          <t>http://monitoreo.datos.gob.ar/catalog/otros/data.json</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t xml:space="preserve">None is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>RESULTADO PROYECTOS</t>
-        </is>
-      </c>
-      <c r="E28" t="b">
-        <v>1</v>
+          <t>GPS Empresas - Discontinuado</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t xml:space="preserve">'superTheme' is a required property &amp;&amp; 'accrualPeriodicity' is a required property &amp;&amp; 'http://www4.hcdn.gob.ar/Datos_doc/DOCUMENTACION – resultado proyectos.pdf' is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="inlineStr">
         <is>
-          <t>https://datos.hcdn.gob.ar/</t>
-        </is>
-      </c>
-      <c r="B29" t="b">
-        <v>1</v>
+          <t>http://monitoreo.datos.gob.ar/catalog/otros/data.json</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t xml:space="preserve">None is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Sesiones</t>
-        </is>
-      </c>
-      <c r="E29" t="b">
-        <v>1</v>
+          <t>Indicadores Sectoriales de Agroindustria - Discontinuado</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t xml:space="preserve">'superTheme' is a required property &amp;&amp; 'http://www4.hcdn.gob.ar/Datos_doc/DOCUMENTACION – SESIONES DESDE 1983.pdf' is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="inlineStr">
         <is>
-          <t>https://datos.hcdn.gob.ar/</t>
-        </is>
-      </c>
-      <c r="B30" t="b">
-        <v>1</v>
+          <t>http://monitoreo.datos.gob.ar/catalog/otros/data.json</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t xml:space="preserve">None is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Subsidios</t>
-        </is>
-      </c>
-      <c r="E30" t="b">
-        <v>1</v>
+          <t>Series de Tiempo vacunas COVID</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t xml:space="preserve">'superTheme' is a required property &amp;&amp; 'accrualPeriodicity' is a required property &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>https://datos.hcdn.gob.ar/</t>
-        </is>
-      </c>
-      <c r="B31" t="b">
-        <v>1</v>
+          <t>http://monitoreo.datos.gob.ar/catalog/otros/data.json</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t xml:space="preserve">None is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Viajes Nacionales</t>
-        </is>
-      </c>
-      <c r="E31" t="b">
-        <v>1</v>
+          <t>REFEGLO - Registro Federal de Gobiernos Locales</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t xml:space="preserve">'superTheme' is a required property &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="inlineStr">
         <is>
-          <t>https://datos.hcdn.gob.ar/</t>
-        </is>
-      </c>
-      <c r="B32" t="b">
-        <v>1</v>
+          <t>https://monitoreo.datos.gob.ar/catalog/modernizacion/data.json</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t xml:space="preserve">None is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Votaciones Nominales</t>
-        </is>
-      </c>
-      <c r="E32" t="b">
-        <v>1</v>
+          <t>Base de Series de Tiempo de la Administración Pública Nacional</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t xml:space="preserve">'superTheme' is a required property &amp;&amp; 'accrualPeriodicity' is a required property &amp;&amp; '' is too short &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="inlineStr">
         <is>
-          <t>https://datos.hcdn.gob.ar/</t>
-        </is>
-      </c>
-      <c r="B33" t="b">
-        <v>1</v>
+          <t>https://monitoreo.datos.gob.ar/catalog/modernizacion/data.json</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t xml:space="preserve">None is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Votaciones Nominales</t>
-        </is>
-      </c>
-      <c r="E33" t="b">
-        <v>1</v>
+          <t>Sistema de Contrataciones Electrónicas</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t xml:space="preserve">'superTheme' is a required property &amp;&amp; 'http://www4.hcdn.gob.ar/Datos_doc/Documentación Votaciones Nominales.pdf' is not valid under any of the given schemas &amp;&amp; </t>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="inlineStr">
+        <is>
+          <t>https://monitoreo.datos.gob.ar/catalog/modernizacion/data.json</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Asignación Salarial de las Autoridades Superiores del Poder Ejecutivo Nacional</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="inlineStr">
+        <is>
+          <t>https://monitoreo.datos.gob.ar/catalog/modernizacion/data.json</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Planes de Apertura de Datos</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="inlineStr">
+        <is>
+          <t>https://monitoreo.datos.gob.ar/catalog/modernizacion/data.json</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Puntos Digitales</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="inlineStr">
+        <is>
+          <t>https://monitoreo.datos.gob.ar/catalog/modernizacion/data.json</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Servicio de normalización de datos geográficos</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="inlineStr">
+        <is>
+          <t>https://monitoreo.datos.gob.ar/catalog/modernizacion/data.json</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Red de Datos Abiertos de la Administración Pública Nacional (APN)</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="inlineStr">
+        <is>
+          <t>https://monitoreo.datos.gob.ar/catalog/modernizacion/data.json</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Nómina del personal civil de la Administración Pública Nacional (APN)</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="inlineStr">
+        <is>
+          <t>https://monitoreo.datos.gob.ar/catalog/modernizacion/data.json</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Puestos de trabajo en la Administración Pública Nacional (APN)</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="inlineStr">
+        <is>
+          <t>https://monitoreo.datos.gob.ar/catalog/modernizacion/data.json</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Contratar</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="inlineStr">
+        <is>
+          <t>https://monitoreo.datos.gob.ar/catalog/modernizacion/data.json</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Puntos WiFi País Digital</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="inlineStr">
+        <is>
+          <t>https://monitoreo.datos.gob.ar/catalog/modernizacion/data.json</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Trámites a Distancia (TAD)</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="inlineStr">
+        <is>
+          <t>https://monitoreo.datos.gob.ar/catalog/modernizacion/data.json</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Tercer Plan de Acción Nacional de Gobierno Abierto</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="inlineStr">
+        <is>
+          <t>https://monitoreo.datos.gob.ar/catalog/modernizacion/data.json</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Indicadores de la Red de Datos Abiertos de la Administración Pública Nacional (APN)</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="inlineStr">
+        <is>
+          <t>https://monitoreo.datos.gob.ar/catalog/smn/data.json</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Prónostico del Tiempo a 5 días</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2" t="inlineStr">
+        <is>
+          <t>https://monitoreo.datos.gob.ar/catalog/smn/data.json</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Datos meteorológicos horarios</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="inlineStr">
+        <is>
+          <t>https://monitoreo.datos.gob.ar/catalog/smn/data.json</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Estado del Tiempo presente</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="inlineStr">
+        <is>
+          <t>https://monitoreo.datos.gob.ar/catalog/smn/data.json</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Observaciones diarias de Temperaturas Extremas</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="inlineStr">
+        <is>
+          <t>https://monitoreo.datos.gob.ar/catalog/smn/data.json</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Registro de Temperatura (365 días)</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="inlineStr">
+        <is>
+          <t>https://monitoreo.datos.gob.ar/catalog/smn/data.json</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Radiación Solar</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="inlineStr">
+        <is>
+          <t>https://monitoreo.datos.gob.ar/catalog/smn/data.json</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Estadísticas Climáticas Normales</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="2" t="inlineStr">
+        <is>
+          <t>https://monitoreo.datos.gob.ar/catalog/smn/data.json</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Listado de Estaciones Meteorológicas del SMN</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -1453,6 +2300,26 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A31" r:id="rId30"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A32" r:id="rId31"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A33" r:id="rId32"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A34" r:id="rId33"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A35" r:id="rId34"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A36" r:id="rId35"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A37" r:id="rId36"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A38" r:id="rId37"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A39" r:id="rId38"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A40" r:id="rId39"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A41" r:id="rId40"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A42" r:id="rId41"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A43" r:id="rId42"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A44" r:id="rId43"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A45" r:id="rId44"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A46" r:id="rId45"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A47" r:id="rId46"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A48" r:id="rId47"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A49" r:id="rId48"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A50" r:id="rId49"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A51" r:id="rId50"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A52" r:id="rId51"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A53" r:id="rId52"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1464,7 +2331,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1480,7 +2347,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Accessible (15/10/2022)</t>
+          <t>Accesible (22/04/2023)</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -1547,28 +2414,30 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>https://datos.hcdn.gob.ar/</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
+          <t>https://transparencia.enargas.gob.ar/data.json</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CKAN</t>
+          <t>Datos abiertos del Ente Nacional Regulador del Gas</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>23</v>
+        <v>267</v>
       </c>
       <c r="E2" t="n">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="F2" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>71</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -1577,7 +2446,7 @@
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>77</v>
+        <v>10</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
@@ -1589,12 +2458,366 @@
         <v>0</v>
       </c>
       <c r="N2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>https://datosabiertos.enacom.gob.ar/data.json</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>no-title</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>https://datos.arsat.com.ar/data.json</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Portal de datos abiertos de ARSAT</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" t="n">
+        <v>8</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>30</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>https://monitoreo.datos.gob.ar/catalog/jgm/data.json</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Datos de la Jefatura de Gabinete de Ministros</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>26</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>8</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>125</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>https://monitoreo.datos.gob.ar/catalog/aaip/data.json</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Datos de la Agencia de Acceso a la Información Pública</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>1169</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>2</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>http://monitoreo.datos.gob.ar/catalog/otros/data.json</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Datos APN</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>-470</v>
+      </c>
+      <c r="E7" t="n">
+        <v>17</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>3</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>136</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>https://monitoreo.datos.gob.ar/catalog/modernizacion/data.json</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Datos Modernización</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>1276</v>
+      </c>
+      <c r="E8" t="n">
+        <v>14</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>8</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>73</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>https://monitoreo.datos.gob.ar/catalog/smn/data.json</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Datos Meteorologicos</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>528</v>
+      </c>
+      <c r="E9" t="n">
+        <v>8</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A2" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A3" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A4" r:id="rId3"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A5" r:id="rId4"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A6" r:id="rId5"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A7" r:id="rId6"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A8" r:id="rId7"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A9" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1606,14 +2829,32 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:W1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Chartpie de % de tipos de distribuciones</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Chartpie de % de dataset erroneos</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>Bar Label de Actualizacion de Accrual Periodicy</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>

</xml_diff>